<commit_message>
Ajout final du TPI
</commit_message>
<xml_diff>
--- a/Documentation/2023.06.02_Nonnenmacher_Enzo_Journal de travail.xlsx
+++ b/Documentation/2023.06.02_Nonnenmacher_Enzo_Journal de travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="112">
   <si>
     <t>Jour</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>Journal de travail</t>
+  </si>
+  <si>
+    <t>Tableau des totaux</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
     <numFmt numFmtId="164" formatCode="hh/mm&quot; h&quot;;@"/>
     <numFmt numFmtId="165" formatCode="[hh]/mm&quot; h&quot;;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,6 +395,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="28"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -401,7 +413,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -409,11 +421,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -461,25 +488,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[hh]/mm&quot; h&quot;;@"/>
     </dxf>
@@ -493,6 +517,15 @@
     <dxf>
       <numFmt numFmtId="21" formatCode="dd/mmm"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -762,12 +795,14 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Totaux!$D$2:$D$6</c:f>
+              <c:f>Totaux!$D$7:$D$11</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -790,7 +825,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Totaux!$E$2:$E$6</c:f>
+              <c:f>Totaux!$E$7:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>[hh]/mm" h";@</c:formatCode>
                 <c:ptCount val="5"/>
@@ -840,6 +875,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -1569,16 +1605,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1607,25 +1643,25 @@
     <tableColumn id="1" name="Jour" dataDxfId="13" totalsRowDxfId="12"/>
     <tableColumn id="2" name="Semaine" dataDxfId="11" totalsRowDxfId="10"/>
     <tableColumn id="3" name="Temps [h]" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="Type" dataDxfId="2" totalsRowDxfId="7"/>
-    <tableColumn id="5" name="Description" dataDxfId="0"/>
-    <tableColumn id="6" name="Commentaire/Remarque/Lien" dataDxfId="1"/>
+    <tableColumn id="4" name="Type" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="5" name="Description" dataDxfId="5"/>
+    <tableColumn id="6" name="Commentaire/Remarque/Lien" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A1:B18" totalsRowCount="1">
-  <autoFilter ref="A1:B17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A6:B23" totalsRowCount="1">
+  <autoFilter ref="A6:B22">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="3">
-      <calculatedColumnFormula>SUM(Journal!C7:C12)</calculatedColumnFormula>
-      <totalsRowFormula>SUM(B2:B17)</totalsRowFormula>
+    <tableColumn id="1" name="Date" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" name="Nb Heures" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0">
+      <calculatedColumnFormula>SUMIF(Tableau1[Jour],A7,Tableau1[Temps '[h']])</calculatedColumnFormula>
+      <totalsRowFormula>SUM(B7:B22)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1897,7 +1933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1912,27 +1948,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -3452,10 +3488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,207 +3501,230 @@
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
         <v>45048</v>
       </c>
-      <c r="B2" s="5">
-        <f>SUMIF(Tableau1[Jour],A2,Tableau1[Temps '[h']])</f>
+      <c r="B7" s="5">
+        <f>SUMIF(Tableau1[Jour],A7,Tableau1[Temps '[h']])</f>
         <v>0.20833333333333331</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D7" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E7" s="22">
         <f>SUMIF(Tableau1[Type],"Analyse",Tableau1[Temps '[h']])</f>
         <v>0.42708333333333326</v>
       </c>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
         <v>45050</v>
       </c>
-      <c r="B3" s="5">
-        <f>SUMIF(Tableau1[Jour],A3,Tableau1[Temps '[h']])</f>
+      <c r="B8" s="5">
+        <f>SUMIF(Tableau1[Jour],A8,Tableau1[Temps '[h']])</f>
         <v>0.21875</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D8" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E8" s="23">
         <f>SUMIF(Tableau1[Type],"Im*",Tableau1[Temps '[h']])</f>
         <v>1.4583333333333335</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
         <v>45051</v>
       </c>
-      <c r="B4" s="5">
-        <f>SUMIF(Tableau1[Jour],A4,Tableau1[Temps '[h']])</f>
+      <c r="B9" s="5">
+        <f>SUMIF(Tableau1[Jour],A9,Tableau1[Temps '[h']])</f>
         <v>0.20833333333333331</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D9" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E9" s="22">
         <f>SUMIF(Tableau1[Type],"Tests",Tableau1[Temps '[h']])</f>
         <v>0.20833333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
         <v>45054</v>
       </c>
-      <c r="B5" s="5">
-        <f>SUMIF(Tableau1[Jour],A5,Tableau1[Temps '[h']])</f>
+      <c r="B10" s="5">
+        <f>SUMIF(Tableau1[Jour],A10,Tableau1[Temps '[h']])</f>
         <v>0.30208333333333326</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D10" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E10" s="23">
         <f>SUMIF(Tableau1[Type],"Documentation",Tableau1[Temps '[h']])</f>
         <v>1.4895833333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>45055</v>
       </c>
-      <c r="B6" s="5">
-        <f>SUMIF(Tableau1[Jour],A6,Tableau1[Temps '[h']])</f>
+      <c r="B11" s="5">
+        <f>SUMIF(Tableau1[Jour],A11,Tableau1[Temps '[h']])</f>
         <v>0.26041666666666669</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D11" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E11" s="23">
         <f>SUMIF(Tableau1[Type],"Divers",Tableau1[Temps '[h']])</f>
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>45057</v>
-      </c>
-      <c r="B7" s="5">
-        <f>SUMIF(Tableau1[Jour],A7,Tableau1[Temps '[h']])</f>
-        <v>0.21875000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>45058</v>
-      </c>
-      <c r="B8" s="5">
-        <f>SUMIF(Tableau1[Jour],A8,Tableau1[Temps '[h']])</f>
-        <v>0.23958333333333334</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>45061</v>
-      </c>
-      <c r="B9" s="5">
-        <f>SUMIF(Tableau1[Jour],A9,Tableau1[Temps '[h']])</f>
-        <v>0.30208333333333331</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>45062</v>
-      </c>
-      <c r="B10" s="5">
-        <f>SUMIF(Tableau1[Jour],A10,Tableau1[Temps '[h']])</f>
-        <v>0.26041666666666663</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>45068</v>
-      </c>
-      <c r="B11" s="5">
-        <f>SUMIF(Tableau1[Jour],A11,Tableau1[Temps '[h']])</f>
-        <v>0.30208333333333331</v>
-      </c>
-    </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
-        <v>45069</v>
+        <v>45057</v>
       </c>
       <c r="B12" s="5">
         <f>SUMIF(Tableau1[Jour],A12,Tableau1[Temps '[h']])</f>
-        <v>0.26041666666666669</v>
+        <v>0.21875000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
-        <v>45071</v>
+        <v>45058</v>
       </c>
       <c r="B13" s="5">
         <f>SUMIF(Tableau1[Jour],A13,Tableau1[Temps '[h']])</f>
-        <v>0.21875</v>
+        <v>0.23958333333333334</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
-        <v>45072</v>
+        <v>45061</v>
       </c>
       <c r="B14" s="5">
         <f>SUMIF(Tableau1[Jour],A14,Tableau1[Temps '[h']])</f>
-        <v>0.23958333333333331</v>
+        <v>0.30208333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
-        <v>45076</v>
+        <v>45062</v>
       </c>
       <c r="B15" s="5">
         <f>SUMIF(Tableau1[Jour],A15,Tableau1[Temps '[h']])</f>
-        <v>0.21875</v>
+        <v>0.26041666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>45078</v>
+        <v>45068</v>
       </c>
       <c r="B16" s="5">
         <f>SUMIF(Tableau1[Jour],A16,Tableau1[Temps '[h']])</f>
-        <v>0.10416666666666666</v>
+        <v>0.30208333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
-        <v>45079</v>
+        <v>45069</v>
       </c>
       <c r="B17" s="5">
         <f>SUMIF(Tableau1[Jour],A17,Tableau1[Temps '[h']])</f>
+        <v>0.26041666666666669</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>45071</v>
+      </c>
+      <c r="B18" s="5">
+        <f>SUMIF(Tableau1[Jour],A18,Tableau1[Temps '[h']])</f>
+        <v>0.21875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>45072</v>
+      </c>
+      <c r="B19" s="5">
+        <f>SUMIF(Tableau1[Jour],A19,Tableau1[Temps '[h']])</f>
+        <v>0.23958333333333331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>45076</v>
+      </c>
+      <c r="B20" s="5">
+        <f>SUMIF(Tableau1[Jour],A20,Tableau1[Temps '[h']])</f>
+        <v>0.21875</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>45078</v>
+      </c>
+      <c r="B21" s="5">
+        <f>SUMIF(Tableau1[Jour],A21,Tableau1[Temps '[h']])</f>
+        <v>0.10416666666666666</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>45079</v>
+      </c>
+      <c r="B22" s="5">
+        <f>SUMIF(Tableau1[Jour],A22,Tableau1[Temps '[h']])</f>
         <v>0.18750000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="12">
-        <f>SUM(B2:B17)</f>
+      <c r="B23" s="12">
+        <f>SUM(B7:B22)</f>
         <v>3.7499999999999996</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>